<commit_message>
Research traker for 360 digit DS/DA internship and Case,When,Then in sql
</commit_message>
<xml_diff>
--- a/Internship_Project/Data Analytics Check list(Raja DS intern Batch 93).xlsx
+++ b/Internship_Project/Data Analytics Check list(Raja DS intern Batch 93).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\360digit DA and DS internship(Batch 93)\Internship_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791D94D2-104C-45C0-8F8D-FE481175FE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C2A868-15A4-454D-B2C3-23EFFC99E7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,49 +578,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">======
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ID#AAAAxC1i8qE
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Sharat    (2023-05-16 06:20:29)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Features could be defined on different scales and might lead to strong bias to features on larger scales, hence normalization is required.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
   <extLst>
     <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion1">
@@ -631,7 +588,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Steps</t>
   </si>
@@ -717,9 +674,6 @@
     <t xml:space="preserve">File format </t>
   </si>
   <si>
-    <t xml:space="preserve">Normalization </t>
-  </si>
-  <si>
     <t xml:space="preserve">Validate performance </t>
   </si>
   <si>
@@ -786,9 +740,6 @@
     <t>Data collected in standard csv file format</t>
   </si>
   <si>
-    <t>To reduce bias range of data is needed</t>
-  </si>
-  <si>
     <t>Python</t>
   </si>
   <si>
@@ -796,6 +747,9 @@
   </si>
   <si>
     <t>Dashboad report will based on the quantitative mesurments in data, describes correlation between measuments to identity machine down time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1188,9 +1142,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W962"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="5" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D36" sqref="D36"/>
+      <selection pane="topRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1330,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1344,7 +1298,7 @@
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1368,7 +1322,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1381,7 +1335,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="10"/>
       <c r="G10" s="4"/>
@@ -1406,7 +1360,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="13"/>
       <c r="G12" s="4"/>
@@ -1419,7 +1373,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -1445,7 +1399,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -1470,7 +1424,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="13"/>
       <c r="G17" s="4"/>
@@ -1483,7 +1437,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="13"/>
       <c r="G18" s="4"/>
@@ -1496,7 +1450,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="13"/>
       <c r="G19" s="4"/>
@@ -1531,7 +1485,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="13"/>
       <c r="G22" s="4"/>
@@ -1555,7 +1509,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="13"/>
       <c r="G24" s="4"/>
@@ -1568,7 +1522,7 @@
         <v>25</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="13"/>
       <c r="G25" s="4"/>
@@ -1592,7 +1546,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="13"/>
       <c r="G27" s="4"/>
@@ -1602,11 +1556,9 @@
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="11" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>51</v>
-      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="13"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1622,7 +1574,7 @@
     </row>
     <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="12"/>
@@ -1632,13 +1584,13 @@
     </row>
     <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E31" s="13"/>
       <c r="G31" s="4"/>
@@ -1655,7 +1607,7 @@
     <row r="33" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="12"/>
@@ -1667,10 +1619,10 @@
       <c r="A34" s="11"/>
       <c r="B34" s="12"/>
       <c r="C34" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E34" s="13"/>
       <c r="G34" s="4"/>
@@ -1688,7 +1640,7 @@
     <row r="36" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="12"/>
@@ -1699,7 +1651,7 @@
     <row r="37" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="12"/>
@@ -1718,10 +1670,10 @@
     </row>
     <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="12"/>

</xml_diff>